<commit_message>
#189, move gfpvan-uat views into demo data.
</commit_message>
<xml_diff>
--- a/pim/src/PcmtCustomDatasetBundle/Resources/fixtures/pcmt_global/import_files/2019-11-29/11_datagrid_view.xlsx
+++ b/pim/src/PcmtCustomDatasetBundle/Resources/fixtures/pcmt_global/import_files/2019-11-29/11_datagrid_view.xlsx
@@ -101,7 +101,7 @@
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>i=1&amp;p=25&amp;s%5BL3%5D=-1&amp;f%5Bfamily%5D%5Bvalue%5D%5B%5D=RH_PRODUCTS_TRADEITEMS_VARIANTS&amp;f%5Bfamily%5D%5Btype%5D=in&amp;f%5Bscope%5D%5Bvalue%5D=channel_product_catalog&amp;f%5Bcategory%5D%5Bvalue%5D%5BtreeId%5D=7&amp;f%5Bcategory%5D%5Bvalue%5D%5BcategoryId%5D=0&amp;f%5Bcategory%5D%5Btype%5D=1&amp;t=product-grid</t>
+          <t>i=1&amp;p=25&amp;s%5BL3%5D=-1&amp;f%5Bfamily%5D%5Bvalue%5D%5B%5D=RH_PRODUCTS_TRADEITEMS_VARIANTS&amp;f%5Bfamily%5D%5Btype%5D=in&amp;f%5Bcategory%5D%5Bvalue%5D%5BtreeId%5D=8&amp;f%5Bcategory%5D%5Bvalue%5D%5BcategoryId%5D=0&amp;f%5Bcategory%5D%5Btype%5D=1&amp;t=product-grid</t>
         </is>
       </c>
       <c r="E2" s="0" t="inlineStr">
@@ -133,7 +133,7 @@
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
-          <t>i=1&amp;p=25&amp;s%5BL3%5D=-1&amp;f%5Bfamily%5D%5Bvalue%5D%5B%5D=RH_PRODUCTS_TRADEITEMS_VARIANTS&amp;f%5Bfamily%5D%5Btype%5D=in&amp;f%5Bscope%5D%5Bvalue%5D=channel_product_catalog&amp;f%5B__L3%5D=1&amp;f%5B__PARENTID%5D=0&amp;f%5B__SOURCEITEMID%5D=1&amp;f%5Bcategory%5D%5Bvalue%5D%5BtreeId%5D=79&amp;f%5Bcategory%5D%5Bvalue%5D%5BcategoryId%5D=0&amp;f%5Bcategory%5D%5Btype%5D=1&amp;t=product-grid</t>
+          <t>i=1&amp;p=25&amp;s%5BL3%5D=-1&amp;f%5Bfamily%5D%5Bvalue%5D%5B%5D=RH_PRODUCTS_TRADEITEMS_VARIANTS&amp;f%5Bfamily%5D%5Btype%5D=in&amp;f%5Bscope%5D%5Bvalue%5D=ecommerce&amp;f%5Bcategory%5D%5Bvalue%5D%5BtreeId%5D=88&amp;f%5Bcategory%5D%5Bvalue%5D%5BcategoryId%5D=0&amp;f%5Bcategory%5D%5Btype%5D=1&amp;t=product-grid</t>
         </is>
       </c>
       <c r="E3" s="0" t="inlineStr">
@@ -165,7 +165,7 @@
       </c>
       <c r="D4" s="0" t="inlineStr">
         <is>
-          <t>i=1&amp;p=25&amp;f%5Bfamily%5D%5Bvalue%5D%5B%5D=GS1_GDSN&amp;f%5Bfamily%5D%5Btype%5D=in&amp;f%5Bscope%5D%5Bvalue%5D=channel_gs1&amp;f%5B__PARENTID%5D=0&amp;f%5Bcategory%5D%5Bvalue%5D%5BtreeId%5D=4&amp;f%5Bcategory%5D%5Bvalue%5D%5BcategoryId%5D=0&amp;f%5Bcategory%5D%5Btype%5D=1&amp;t=product-grid</t>
+          <t>i=1&amp;p=25&amp;s%5Bupdated%5D=1&amp;f%5Bfamily%5D%5Bvalue%5D%5B%5D=GS1_GDSN&amp;f%5Bfamily%5D%5Btype%5D=in&amp;f%5Bscope%5D%5Bvalue%5D=GS1_GDSN&amp;f%5Bcategory%5D%5Bvalue%5D%5BtreeId%5D=4&amp;f%5Bcategory%5D%5Bvalue%5D%5BcategoryId%5D=0&amp;f%5Bcategory%5D%5Btype%5D=1&amp;t=product-grid</t>
         </is>
       </c>
       <c r="E4" s="0" t="inlineStr">
@@ -197,7 +197,7 @@
       </c>
       <c r="D5" s="0" t="inlineStr">
         <is>
-          <t>i=1&amp;p=25&amp;s%5Bupdated%5D=1&amp;f%5Bfamily%5D%5Bvalue%5D%5B%5D=MD_RECIPIENT_MAPPING&amp;f%5Bfamily%5D%5Btype%5D=in&amp;f%5Bscope%5D%5Bvalue%5D=channel_product_catalog&amp;f%5Bcategory%5D%5Bvalue%5D%5BtreeId%5D=1&amp;f%5Bcategory%5D%5Bvalue%5D%5BcategoryId%5D=3&amp;f%5Bcategory%5D%5Btype%5D=1&amp;t=product-grid</t>
+          <t>i=1&amp;p=25&amp;s%5Bupdated%5D=1&amp;f%5Bfamily%5D%5Bvalue%5D%5B%5D=MD_RECIPIENT_MAPPING&amp;f%5Bfamily%5D%5Btype%5D=in&amp;f%5Bscope%5D%5Bvalue%5D=ecommerce&amp;f%5Bcategory%5D%5Bvalue%5D%5BtreeId%5D=1&amp;f%5Bcategory%5D%5Bvalue%5D%5BcategoryId%5D=3&amp;f%5Bcategory%5D%5Btype%5D=1&amp;t=product-grid</t>
         </is>
       </c>
       <c r="E5" s="0" t="inlineStr">
@@ -229,7 +229,7 @@
       </c>
       <c r="D6" s="0" t="inlineStr">
         <is>
-          <t>i=1&amp;p=25&amp;s%5Bupdated%5D=1&amp;f%5Bfamily%5D%5Bvalue%5D%5B%5D=MD_SUPPLIER_MAPPING&amp;f%5Bfamily%5D%5Btype%5D=in&amp;f%5Bscope%5D%5Bvalue%5D=channel_product_catalog&amp;f%5Bcategory%5D%5Bvalue%5D%5BtreeId%5D=1&amp;f%5Bcategory%5D%5Bvalue%5D%5BcategoryId%5D=3&amp;f%5Bcategory%5D%5Btype%5D=1&amp;t=product-grid</t>
+          <t>i=1&amp;p=25&amp;s%5Bupdated%5D=1&amp;f%5Bfamily%5D%5Bvalue%5D%5B%5D=MD_SUPPLIER_MAPPING&amp;f%5Bfamily%5D%5Btype%5D=in&amp;f%5Bscope%5D%5Bvalue%5D=ecommerce&amp;f%5Bcategory%5D%5Bvalue%5D%5BtreeId%5D=1&amp;f%5Bcategory%5D%5Bvalue%5D%5BcategoryId%5D=3&amp;f%5Bcategory%5D%5Btype%5D=1&amp;t=product-grid</t>
         </is>
       </c>
       <c r="E6" s="0" t="inlineStr">
@@ -261,7 +261,7 @@
       </c>
       <c r="D7" s="0" t="inlineStr">
         <is>
-          <t>i=3&amp;p=25&amp;s%5Bupdated%5D=1&amp;f%5Bfamily%5D%5Bvalue%5D%5B%5D=MD_SUPPLIER_MASTER&amp;f%5Bfamily%5D%5Btype%5D=in&amp;f%5Bscope%5D%5Bvalue%5D=channel_product_catalog&amp;f%5Bcategory%5D%5Bvalue%5D%5BtreeId%5D=1&amp;f%5Bcategory%5D%5Bvalue%5D%5BcategoryId%5D=3&amp;f%5Bcategory%5D%5Btype%5D=1&amp;t=product-grid</t>
+          <t>i=1&amp;p=25&amp;s%5Bupdated%5D=1&amp;f%5Bfamily%5D%5Bvalue%5D%5B%5D=MD_SUPPLIER_MASTER&amp;f%5Bfamily%5D%5Btype%5D=in&amp;f%5Bscope%5D%5Bvalue%5D=ecommerce&amp;f%5Bcategory%5D%5Bvalue%5D%5BtreeId%5D=1&amp;f%5Bcategory%5D%5Bvalue%5D%5BcategoryId%5D=3&amp;f%5Bcategory%5D%5Btype%5D=1&amp;t=product-grid</t>
         </is>
       </c>
       <c r="E7" s="0" t="inlineStr">
@@ -293,7 +293,7 @@
       </c>
       <c r="D8" s="0" t="inlineStr">
         <is>
-          <t>i=1&amp;p=25&amp;s%5Bupdated%5D=1&amp;f%5Bfamily%5D%5Bvalue%5D%5B%5D=MD_HUB&amp;f%5Bfamily%5D%5Btype%5D=in&amp;f%5Bscope%5D%5Bvalue%5D=channel_product_catalog&amp;f%5Bcategory%5D%5Bvalue%5D%5BtreeId%5D=1&amp;f%5Bcategory%5D%5Bvalue%5D%5BcategoryId%5D=3&amp;f%5Bcategory%5D%5Btype%5D=1&amp;t=product-grid</t>
+          <t>i=1&amp;p=25&amp;s%5BMD_HUB_GLOBAL_ENTERPRISE_ID%5D=-1&amp;f%5Bfamily%5D%5Bvalue%5D%5B%5D=MD_HUB&amp;f%5Bfamily%5D%5Btype%5D=in&amp;f%5Bscope%5D%5Bvalue%5D=PRODUCT_CATALOG&amp;f%5Bcategory%5D%5Bvalue%5D%5BtreeId%5D=1&amp;f%5Bcategory%5D%5Bvalue%5D%5BcategoryId%5D=3&amp;f%5Bcategory%5D%5Btype%5D=1&amp;t=product-grid</t>
         </is>
       </c>
       <c r="E8" s="0" t="inlineStr">
@@ -334,6 +334,38 @@
         </is>
       </c>
       <c r="F9" s="0" t="inlineStr">
+        <is>
+          <t>public</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="0" t="inlineStr">
+        <is>
+          <t>UNASSIGNED PRODUCTS AND ITEMS</t>
+        </is>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>updated,MD_SUPPLIER_MASTER_SUPPLIERID,MD_SUPPLIER_MASTER_SUPPLIERNAME,MD_SUPPLIER_MASTER_ALIASES,MD_SUPPLIER_MASTER_SUPPLIER_SITE,MD_SUPPLIER_MASTER_GLN</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>product-grid</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>i=1&amp;p=25&amp;s%5Bupdated%5D=1&amp;f%5Bscope%5D%5Bvalue%5D=PRODUCT_CATALOG&amp;f%5Bcategory%5D%5Bvalue%5D%5BtreeId%5D=1&amp;f%5Bcategory%5D%5Bvalue%5D%5BcategoryId%5D=-1&amp;f%5Bcategory%5D%5Btype%5D=1&amp;t=product-grid</t>
+        </is>
+      </c>
+      <c r="E10" s="0" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="F10" s="0" t="inlineStr">
         <is>
           <t>public</t>
         </is>

</xml_diff>